<commit_message>
revisi: ubah export menjadi 3 dan tambahkan fitur upload image pada beranda(auth)
</commit_message>
<xml_diff>
--- a/assets/document/data-latih/Book1.xlsx
+++ b/assets/document/data-latih/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arlan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BE8C396-87A4-480E-A628-66D2BC1DA757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56FE8459-2651-44FC-A9E0-5CC34EFB45DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24045" yWindow="-1920" windowWidth="20700" windowHeight="11565" xr2:uid="{50BDED58-6943-435A-8661-E219452A30B4}"/>
+    <workbookView xWindow="-26475" yWindow="-1800" windowWidth="20700" windowHeight="11565" xr2:uid="{28F501EC-74D9-4068-B20E-8BBDD952D50D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCE0798-8B00-418C-8015-C52D8E1D8C51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4617F9DC-02E4-4767-A69F-E987C17C12C9}">
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">

</xml_diff>